<commit_message>
configured scripts to run in maven fw
</commit_message>
<xml_diff>
--- a/src/test/java/dataEngine/DataEngine.xlsx
+++ b/src/test/java/dataEngine/DataEngine.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="339">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1032,13 +1032,10 @@
     <t>*Note: Closed and FieldComp not in the list of status change when WO is in Create status - this is the correct functionality but it's not the case in TST environment and it is in UAT</t>
   </si>
   <si>
-    <t>PASS</t>
+    <t>Yes</t>
   </si>
   <si>
     <t>FAIL</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -1524,8 +1521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,10 +1604,10 @@
         <v>6</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="8" t="s">
         <v>337</v>
+      </c>
+      <c r="E4" t="s">
+        <v>338</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>321</v>
@@ -1633,9 +1630,7 @@
       <c r="D5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>337</v>
-      </c>
+      <c r="E5" s="8"/>
       <c r="F5" s="13" t="s">
         <v>321</v>
       </c>
@@ -1677,9 +1672,6 @@
       <c r="D7" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E7" t="s">
-        <v>337</v>
-      </c>
       <c r="F7" s="13" t="s">
         <v>321</v>
       </c>
@@ -1701,9 +1693,6 @@
       <c r="D8" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E8" t="s">
-        <v>337</v>
-      </c>
       <c r="F8" s="13" t="s">
         <v>321</v>
       </c>
@@ -1725,9 +1714,6 @@
       <c r="D9" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E9" t="s">
-        <v>337</v>
-      </c>
       <c r="F9" s="13" t="s">
         <v>321</v>
       </c>
@@ -1770,9 +1756,6 @@
       <c r="D11" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E11" t="s">
-        <v>337</v>
-      </c>
       <c r="F11" s="13" t="s">
         <v>321</v>
       </c>
@@ -1850,9 +1833,6 @@
       <c r="D15" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E15" t="s">
-        <v>337</v>
-      </c>
       <c r="F15" s="13" t="s">
         <v>321</v>
       </c>
@@ -1932,9 +1912,6 @@
       <c r="D19" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E19" t="s">
-        <v>337</v>
-      </c>
       <c r="F19" s="13" t="s">
         <v>321</v>
       </c>
@@ -1956,9 +1933,6 @@
       <c r="D20" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E20" t="s">
-        <v>337</v>
-      </c>
       <c r="F20" s="13" t="s">
         <v>321</v>
       </c>
@@ -1980,9 +1954,6 @@
       <c r="D21" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E21" t="s">
-        <v>337</v>
-      </c>
       <c r="F21" s="13" t="s">
         <v>321</v>
       </c>
@@ -2002,9 +1973,6 @@
       <c r="D22" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E22" t="s">
-        <v>337</v>
-      </c>
       <c r="F22" s="13" t="s">
         <v>321</v>
       </c>
@@ -2025,9 +1993,6 @@
       </c>
       <c r="D23" s="24" t="s">
         <v>5</v>
-      </c>
-      <c r="E23" t="s">
-        <v>337</v>
       </c>
       <c r="F23" s="13" t="s">
         <v>321</v>
@@ -2070,9 +2035,6 @@
       <c r="D25" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E25" t="s">
-        <v>337</v>
-      </c>
       <c r="F25" s="13" t="s">
         <v>321</v>
       </c>
@@ -2116,9 +2078,6 @@
       <c r="D27" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E27" t="s">
-        <v>337</v>
-      </c>
       <c r="F27" s="13" t="s">
         <v>321</v>
       </c>
@@ -2140,9 +2099,6 @@
       <c r="D28" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E28" t="s">
-        <v>337</v>
-      </c>
       <c r="F28" s="13" t="s">
         <v>321</v>
       </c>
@@ -2186,9 +2142,6 @@
       <c r="D30" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E30" t="s">
-        <v>337</v>
-      </c>
       <c r="F30" s="13" t="s">
         <v>321</v>
       </c>
@@ -2212,9 +2165,6 @@
       <c r="D31" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E31" t="s">
-        <v>337</v>
-      </c>
       <c r="F31" s="13" t="s">
         <v>321</v>
       </c>
@@ -2235,9 +2185,6 @@
       </c>
       <c r="D32" s="24" t="s">
         <v>5</v>
-      </c>
-      <c r="E32" t="s">
-        <v>337</v>
       </c>
       <c r="F32" s="13" t="s">
         <v>321</v>
@@ -2400,9 +2347,6 @@
       <c r="D40" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E40" t="s">
-        <v>337</v>
-      </c>
       <c r="F40" s="13" t="s">
         <v>321</v>
       </c>
@@ -2421,10 +2365,7 @@
         <v>68</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>339</v>
-      </c>
-      <c r="E41" t="s">
-        <v>338</v>
+        <v>5</v>
       </c>
       <c r="F41" s="13" t="s">
         <v>321</v>
@@ -2447,9 +2388,6 @@
       <c r="D42" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E42" t="s">
-        <v>337</v>
-      </c>
       <c r="F42" s="13" t="s">
         <v>321</v>
       </c>
@@ -2470,9 +2408,6 @@
       <c r="D43" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E43" t="s">
-        <v>337</v>
-      </c>
       <c r="F43" s="13" t="s">
         <v>321</v>
       </c>
@@ -2493,9 +2428,6 @@
       <c r="D44" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E44" t="s">
-        <v>337</v>
-      </c>
       <c r="F44" s="13" t="s">
         <v>321</v>
       </c>
@@ -2518,9 +2450,6 @@
       <c r="D45" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E45" t="s">
-        <v>337</v>
-      </c>
       <c r="F45" s="13" t="s">
         <v>321</v>
       </c>
@@ -2538,9 +2467,6 @@
       <c r="D46" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E46" t="s">
-        <v>337</v>
-      </c>
       <c r="F46" s="13" t="s">
         <v>321</v>
       </c>
@@ -2573,9 +2499,6 @@
       <c r="D48" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E48" t="s">
-        <v>337</v>
-      </c>
       <c r="F48" s="13" t="s">
         <v>321</v>
       </c>
@@ -2593,9 +2516,6 @@
       <c r="D49" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E49" t="s">
-        <v>337</v>
-      </c>
       <c r="F49" s="13" t="s">
         <v>321</v>
       </c>
@@ -2633,9 +2553,6 @@
       <c r="D51" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E51" t="s">
-        <v>337</v>
-      </c>
       <c r="F51" s="13" t="s">
         <v>321</v>
       </c>
@@ -2651,9 +2568,6 @@
       <c r="D52" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E52" t="s">
-        <v>337</v>
-      </c>
       <c r="F52" s="13" t="s">
         <v>321</v>
       </c>
@@ -2669,9 +2583,6 @@
       <c r="D53" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E53" t="s">
-        <v>337</v>
-      </c>
       <c r="F53" s="13" t="s">
         <v>321</v>
       </c>
@@ -2687,9 +2598,6 @@
       <c r="D54" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E54" t="s">
-        <v>337</v>
-      </c>
       <c r="F54" s="13" t="s">
         <v>321</v>
       </c>
@@ -2705,9 +2613,6 @@
       <c r="D55" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E55" t="s">
-        <v>337</v>
-      </c>
       <c r="F55" s="13" t="s">
         <v>321</v>
       </c>
@@ -2723,9 +2628,6 @@
       <c r="D56" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E56" t="s">
-        <v>337</v>
-      </c>
       <c r="F56" s="13" t="s">
         <v>321</v>
       </c>
@@ -2743,9 +2645,6 @@
       <c r="D57" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E57" t="s">
-        <v>337</v>
-      </c>
       <c r="F57" s="13" t="s">
         <v>321</v>
       </c>
@@ -2764,9 +2663,6 @@
       <c r="D58" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E58" t="s">
-        <v>337</v>
-      </c>
       <c r="F58" s="13" t="s">
         <v>321</v>
       </c>
@@ -2784,9 +2680,6 @@
       <c r="D59" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E59" t="s">
-        <v>337</v>
-      </c>
       <c r="F59" s="13" t="s">
         <v>321</v>
       </c>
@@ -2804,9 +2697,6 @@
       <c r="D60" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E60" t="s">
-        <v>337</v>
-      </c>
       <c r="F60" s="13" t="s">
         <v>321</v>
       </c>
@@ -2824,9 +2714,6 @@
       <c r="D61" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E61" t="s">
-        <v>337</v>
-      </c>
       <c r="F61" s="13" t="s">
         <v>321</v>
       </c>
@@ -2847,9 +2734,6 @@
       <c r="D62" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E62" t="s">
-        <v>337</v>
-      </c>
       <c r="F62" s="13" t="s">
         <v>321</v>
       </c>
@@ -2868,9 +2752,6 @@
       <c r="D63" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E63" t="s">
-        <v>337</v>
-      </c>
       <c r="F63" s="13" t="s">
         <v>321</v>
       </c>
@@ -2889,9 +2770,6 @@
       <c r="D64" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E64" t="s">
-        <v>337</v>
-      </c>
       <c r="F64" s="13" t="s">
         <v>321</v>
       </c>
@@ -2910,9 +2788,6 @@
       <c r="D65" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E65" t="s">
-        <v>337</v>
-      </c>
       <c r="F65" s="13" t="s">
         <v>321</v>
       </c>
@@ -2963,9 +2838,6 @@
       <c r="D68" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E68" t="s">
-        <v>337</v>
-      </c>
       <c r="F68" s="13" t="s">
         <v>321</v>
       </c>
@@ -2983,9 +2855,6 @@
       <c r="D69" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E69" t="s">
-        <v>337</v>
-      </c>
       <c r="F69" s="13" t="s">
         <v>321</v>
       </c>
@@ -3003,9 +2872,6 @@
       <c r="D70" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E70" t="s">
-        <v>337</v>
-      </c>
       <c r="F70" s="13" t="s">
         <v>321</v>
       </c>
@@ -3026,9 +2892,6 @@
       <c r="D71" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E71" t="s">
-        <v>337</v>
-      </c>
       <c r="F71" s="13" t="s">
         <v>321</v>
       </c>
@@ -3046,9 +2909,6 @@
       <c r="D72" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E72" t="s">
-        <v>337</v>
-      </c>
       <c r="F72" s="13" t="s">
         <v>321</v>
       </c>
@@ -3756,9 +3616,6 @@
       <c r="D113" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E113" t="s">
-        <v>337</v>
-      </c>
       <c r="F113" s="13" t="s">
         <v>321</v>
       </c>
@@ -3810,9 +3667,6 @@
       <c r="D116" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E116" t="s">
-        <v>337</v>
-      </c>
       <c r="F116" s="13" t="s">
         <v>321</v>
       </c>
@@ -3828,9 +3682,6 @@
       <c r="D117" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E117" t="s">
-        <v>337</v>
-      </c>
       <c r="F117" s="13" t="s">
         <v>321</v>
       </c>
@@ -3848,9 +3699,6 @@
       <c r="D118" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E118" t="s">
-        <v>337</v>
-      </c>
       <c r="F118" s="13" t="s">
         <v>321</v>
       </c>
@@ -3868,9 +3716,6 @@
       <c r="D119" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E119" t="s">
-        <v>337</v>
-      </c>
       <c r="F119" s="13" t="s">
         <v>321</v>
       </c>
@@ -3888,9 +3733,6 @@
       <c r="D120" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E120" t="s">
-        <v>337</v>
-      </c>
       <c r="F120" s="13" t="s">
         <v>321</v>
       </c>
@@ -3906,9 +3748,6 @@
       <c r="D121" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E121" t="s">
-        <v>337</v>
-      </c>
       <c r="F121" s="13" t="s">
         <v>321</v>
       </c>
@@ -3926,9 +3765,6 @@
       <c r="D122" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E122" t="s">
-        <v>337</v>
-      </c>
       <c r="F122" s="13" t="s">
         <v>321</v>
       </c>
@@ -3946,9 +3782,6 @@
       <c r="D123" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E123" t="s">
-        <v>337</v>
-      </c>
       <c r="F123" s="13" t="s">
         <v>321</v>
       </c>
@@ -3966,9 +3799,6 @@
       <c r="D124" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E124" t="s">
-        <v>337</v>
-      </c>
       <c r="F124" s="13" t="s">
         <v>321</v>
       </c>
@@ -3986,9 +3816,6 @@
       <c r="D125" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E125" t="s">
-        <v>338</v>
-      </c>
       <c r="F125" s="13" t="s">
         <v>321</v>
       </c>
@@ -4006,9 +3833,6 @@
       <c r="D126" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E126" t="s">
-        <v>337</v>
-      </c>
       <c r="F126" s="13" t="s">
         <v>321</v>
       </c>
@@ -4026,9 +3850,6 @@
       <c r="D127" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E127" t="s">
-        <v>338</v>
-      </c>
       <c r="F127" s="13" t="s">
         <v>321</v>
       </c>
@@ -4049,9 +3870,6 @@
       <c r="D128" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E128" t="s">
-        <v>337</v>
-      </c>
       <c r="F128" s="13" t="s">
         <v>321</v>
       </c>
@@ -4139,9 +3957,6 @@
       <c r="D133" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E133" t="s">
-        <v>337</v>
-      </c>
       <c r="F133" s="13" t="s">
         <v>321</v>
       </c>
@@ -4158,9 +3973,6 @@
       </c>
       <c r="D134" s="24" t="s">
         <v>5</v>
-      </c>
-      <c r="E134" t="s">
-        <v>337</v>
       </c>
       <c r="F134" s="13" t="s">
         <v>321</v>

</xml_diff>